<commit_message>
New function, get_from_excel, which is in line with how PAM wants its data
</commit_message>
<xml_diff>
--- a/PCA/PCA_test.xlsx
+++ b/PCA/PCA_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eirik\Documents\CDIO\Kod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linus/Desktop/TATA62/PCA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292925D1-452D-43C6-A8A2-001269048B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75553003-0A47-8648-81B9-60D0C1FA2249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E9A40D9F-703E-474E-91FE-C64FC4383DDE}"/>
+    <workbookView xWindow="8540" yWindow="0" windowWidth="27300" windowHeight="22400" xr2:uid="{E9A40D9F-703E-474E-91FE-C64FC4383DDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Cash Flows" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Cash flow</t>
   </si>
@@ -44,15 +44,26 @@
     <t>T</t>
   </si>
   <si>
-    <t>Idag</t>
+    <t>Dagens datum</t>
+  </si>
+  <si>
+    <t>Slutdatum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -68,7 +79,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -76,13 +87,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -101,7 +122,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -397,97 +418,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48199DFD-D728-4D76-B9B6-690398A8085D}">
-  <dimension ref="C4:Z29"/>
+  <dimension ref="C5:X29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="4.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="26" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="26" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:26" x14ac:dyDescent="0.35">
-      <c r="G4" t="s">
+    <row r="5" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C5" s="1"/>
+      <c r="E5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="3:26" x14ac:dyDescent="0.35">
-      <c r="C5" s="1"/>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>44852</v>
-      </c>
-      <c r="H5" s="1">
-        <v>44853</v>
-      </c>
-      <c r="I5" s="1">
-        <v>44854</v>
-      </c>
-      <c r="J5" s="1">
-        <v>44855</v>
-      </c>
-      <c r="K5" s="1">
-        <v>44856</v>
-      </c>
-      <c r="L5" s="1">
-        <v>44857</v>
-      </c>
-      <c r="M5" s="1">
-        <v>44858</v>
-      </c>
-      <c r="N5" s="1">
-        <v>44859</v>
-      </c>
-      <c r="O5" s="1">
-        <v>44860</v>
-      </c>
-      <c r="P5" s="1">
-        <v>44861</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>44862</v>
-      </c>
-      <c r="R5" s="1">
-        <v>44863</v>
-      </c>
-      <c r="S5" s="1">
-        <v>44864</v>
-      </c>
-      <c r="T5" s="1">
-        <v>44865</v>
-      </c>
-      <c r="U5" s="1">
-        <v>44866</v>
-      </c>
-      <c r="V5" s="1">
-        <v>44867</v>
-      </c>
-      <c r="W5" s="1">
-        <v>44868</v>
-      </c>
-      <c r="X5" s="1">
-        <v>44869</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>44870</v>
-      </c>
-      <c r="Z5" s="1">
-        <v>44871</v>
-      </c>
-    </row>
-    <row r="6" spans="3:26" x14ac:dyDescent="0.35">
+      <c r="H5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C6" s="1"/>
       <c r="E6" s="1">
         <v>44917</v>
@@ -495,88 +457,14 @@
       <c r="F6">
         <v>100</v>
       </c>
-      <c r="G6">
-        <f>($E6-G$5)/365</f>
-        <v>0.17808219178082191</v>
-      </c>
-      <c r="H6">
-        <f t="shared" ref="H6:Z7" si="0">($E6-H$5)/365</f>
-        <v>0.17534246575342466</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>0.17260273972602741</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>0.16986301369863013</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>0.16712328767123288</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="0"/>
-        <v>0.16438356164383561</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="0"/>
-        <v>0.16164383561643836</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="0"/>
-        <v>0.15890410958904111</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="0"/>
-        <v>0.15616438356164383</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="0"/>
-        <v>0.15342465753424658</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="0"/>
-        <v>0.15068493150684931</v>
-      </c>
-      <c r="R6">
-        <f t="shared" si="0"/>
-        <v>0.14794520547945206</v>
-      </c>
-      <c r="S6">
-        <f t="shared" si="0"/>
-        <v>0.14520547945205478</v>
-      </c>
-      <c r="T6">
-        <f t="shared" si="0"/>
-        <v>0.14246575342465753</v>
-      </c>
-      <c r="U6">
-        <f t="shared" si="0"/>
-        <v>0.13972602739726028</v>
-      </c>
-      <c r="V6">
-        <f t="shared" si="0"/>
-        <v>0.13698630136986301</v>
-      </c>
-      <c r="W6">
-        <f t="shared" si="0"/>
-        <v>0.13424657534246576</v>
-      </c>
-      <c r="X6">
-        <f t="shared" si="0"/>
-        <v>0.13150684931506848</v>
-      </c>
-      <c r="Y6">
-        <f t="shared" si="0"/>
-        <v>0.12876712328767123</v>
-      </c>
-      <c r="Z6">
-        <f t="shared" si="0"/>
-        <v>0.12602739726027398</v>
-      </c>
-    </row>
-    <row r="7" spans="3:26" x14ac:dyDescent="0.35">
+      <c r="G6" s="1">
+        <v>44852</v>
+      </c>
+      <c r="H6" s="1">
+        <v>44871</v>
+      </c>
+    </row>
+    <row r="7" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C7" s="1"/>
       <c r="E7" s="1">
         <v>44927</v>
@@ -584,151 +472,91 @@
       <c r="F7">
         <v>200</v>
       </c>
-      <c r="G7">
-        <f>($E7-G$5)/365</f>
-        <v>0.20547945205479451</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
-        <v>0.20273972602739726</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
-        <v>0.19726027397260273</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
-        <v>0.19452054794520549</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="0"/>
-        <v>0.19178082191780821</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="0"/>
-        <v>0.18904109589041096</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="0"/>
-        <v>0.18630136986301371</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="0"/>
-        <v>0.18356164383561643</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="0"/>
-        <v>0.18082191780821918</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="0"/>
-        <v>0.17808219178082191</v>
-      </c>
-      <c r="R7">
-        <f t="shared" si="0"/>
-        <v>0.17534246575342466</v>
-      </c>
-      <c r="S7">
-        <f t="shared" si="0"/>
-        <v>0.17260273972602741</v>
-      </c>
-      <c r="T7">
-        <f t="shared" si="0"/>
-        <v>0.16986301369863013</v>
-      </c>
-      <c r="U7">
-        <f t="shared" si="0"/>
-        <v>0.16712328767123288</v>
-      </c>
-      <c r="V7">
-        <f t="shared" si="0"/>
-        <v>0.16438356164383561</v>
-      </c>
-      <c r="W7">
-        <f t="shared" si="0"/>
-        <v>0.16164383561643836</v>
-      </c>
-      <c r="X7">
-        <f t="shared" si="0"/>
-        <v>0.15890410958904111</v>
-      </c>
-      <c r="Y7">
-        <f t="shared" si="0"/>
-        <v>0.15616438356164383</v>
-      </c>
-      <c r="Z7">
-        <f t="shared" si="0"/>
-        <v>0.15342465753424658</v>
-      </c>
-    </row>
-    <row r="8" spans="3:26" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="3:26" x14ac:dyDescent="0.35">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+    </row>
+    <row r="12" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C29" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uppdaterad excel to matlab
</commit_message>
<xml_diff>
--- a/PCA/PCA_test.xlsx
+++ b/PCA/PCA_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linus/Desktop/TATA62/PCA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/024efd841f36a2c5/Skrivbord/TATA62/profit_decomposition/PCA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75553003-0A47-8648-81B9-60D0C1FA2249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{75553003-0A47-8648-81B9-60D0C1FA2249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{363C4DE6-A68A-41B0-80D8-F36116EBE828}"/>
   <bookViews>
-    <workbookView xWindow="8540" yWindow="0" windowWidth="27300" windowHeight="22400" xr2:uid="{E9A40D9F-703E-474E-91FE-C64FC4383DDE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E9A40D9F-703E-474E-91FE-C64FC4383DDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Cash Flows" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>Cash flow</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Slutdatum</t>
+  </si>
+  <si>
+    <t>Cashflow</t>
   </si>
 </sst>
 </file>
@@ -421,20 +424,24 @@
   <dimension ref="C5:X29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="26" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="26" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="E5" s="2" t="s">
         <v>1</v>
@@ -448,8 +455,20 @@
       <c r="H5" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O5" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
       <c r="E6" s="1">
         <v>44917</v>
@@ -463,8 +482,20 @@
       <c r="H6" s="1">
         <v>44871</v>
       </c>
-    </row>
-    <row r="7" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="M6" s="1">
+        <v>44854</v>
+      </c>
+      <c r="N6">
+        <v>100</v>
+      </c>
+      <c r="O6" s="1">
+        <v>44852</v>
+      </c>
+      <c r="P6" s="1">
+        <v>44871</v>
+      </c>
+    </row>
+    <row r="7" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="E7" s="1">
         <v>44927</v>
@@ -472,17 +503,23 @@
       <c r="F7">
         <v>200</v>
       </c>
-    </row>
-    <row r="8" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="M7" s="1">
+        <v>44927</v>
+      </c>
+      <c r="N7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -505,58 +542,58 @@
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
     </row>
-    <row r="12" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
     </row>
   </sheetData>

</xml_diff>